<commit_message>
changed topic model plus to include words length 3 and up. Fixed stopwords for ICS. Initial trend analysis results are in the notebook
</commit_message>
<xml_diff>
--- a/output data/hazard_interpretation_v2.xlsx
+++ b/output data/hazard_interpretation_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\output data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10C47CF-625D-4FFB-924C-B06FD4F4EC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B452C8-9E5F-4F7F-896F-9CE7D72F2007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15132" yWindow="1284" windowWidth="17280" windowHeight="10044" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
+    <workbookView xWindow="1680" yWindow="996" windowWidth="17280" windowHeight="10044" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hazard-focused" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="210">
   <si>
     <t>Hazard level 1 topics</t>
   </si>
@@ -319,12 +319,6 @@
     <t>4, 72</t>
   </si>
   <si>
-    <t>jurisdictions, team, ommand, organization, type</t>
-  </si>
-  <si>
-    <t>involved, transition, transfer</t>
-  </si>
-  <si>
     <t>mixed/general</t>
   </si>
   <si>
@@ -346,9 +340,6 @@
     <t>grazing, pasture, threaten, concern, risk, threat</t>
   </si>
   <si>
-    <t>evacuation, evacuate,  threaten, threat</t>
-  </si>
-  <si>
     <t>mixed, some endangered species</t>
   </si>
   <si>
@@ -361,12 +352,6 @@
     <t>mixed, some weather, not necessarily the hazards we want</t>
   </si>
   <si>
-    <t>weather, behavior, wind, thunderstorm, storm, gusty, lightning</t>
-  </si>
-  <si>
-    <t>unpredictable, extreme, erratic, strong</t>
-  </si>
-  <si>
     <t>mixed/demob</t>
   </si>
   <si>
@@ -448,9 +433,6 @@
     <t>narrow, hazard, snag, create, heavy, fuel, material, community gulch idlewild, terrian, roll, road, advisory, steep, prevail, emergency, terrain, adobe, dense</t>
   </si>
   <si>
-    <t>terrain, rollout, snag, steep, debris, access, terrian</t>
-  </si>
-  <si>
     <t>concern, hazardous, pose, heavy, rugged, difficult, steep, narrow</t>
   </si>
   <si>
@@ -502,18 +484,12 @@
     <t>mixed, possible website information for stake holders</t>
   </si>
   <si>
-    <t>political, social, adjacent, community, cultural, tribal, monument</t>
-  </si>
-  <si>
     <t>weather, not hazardous, humidity, etc</t>
   </si>
   <si>
     <t>low, humidity, relative, temperature, fuel, moisture, extreme, weather, windy, condition, heat, moderate</t>
   </si>
   <si>
-    <t>low, dry</t>
-  </si>
-  <si>
     <t>mixed, some habitat stuff, redundant</t>
   </si>
   <si>
@@ -532,12 +508,6 @@
     <t>mixed, injury, habitats, etc</t>
   </si>
   <si>
-    <t>injury, hospital, injured, accident, treatment, laceration, firefighter, treated</t>
-  </si>
-  <si>
-    <t>minor, report, transport, heat, shoulder, ankle, medical, released</t>
-  </si>
-  <si>
     <t>weather related, redundant</t>
   </si>
   <si>
@@ -553,9 +523,6 @@
     <t>mixed, some weather some general</t>
   </si>
   <si>
-    <t>humidity, moisture, hot</t>
-  </si>
-  <si>
     <t>general firefighting, low quality</t>
   </si>
   <si>
@@ -577,31 +544,127 @@
     <t>infrastructure, utility, powerline, water, electric, pipeline, powerlines, watershed, pole, power, gas</t>
   </si>
   <si>
-    <t>species, specie, habitat, animal, plant, conservation</t>
-  </si>
-  <si>
-    <t>threaten, endanger, threat, sensitive, threatened, endangered, risk, loss, impacts</t>
-  </si>
-  <si>
-    <t>resident,  residence, level, notice, community, structure, subdivision, mandatory, order, effect, remain, continue, issued, issue</t>
-  </si>
-  <si>
     <t>closure, remain, remains, close, block, continue, impact, access, limit, limited</t>
   </si>
   <si>
     <t>lack, need, shortage, minimal, share, necessary, limited, limit, fatigue</t>
   </si>
   <si>
-    <t>unstaffed, resources, support, crew, aircraft, helicopter, engines, staffing, staff</t>
-  </si>
-  <si>
     <t>aircraft, heli, helicopter, aerial, tanker, copter</t>
   </si>
   <si>
-    <t>grounded, ground, suspended, suspend, smoke, impact, hazard</t>
-  </si>
-  <si>
     <t>resume</t>
+  </si>
+  <si>
+    <t>weather, behavior, wind, thunderstorm, storm, gusty, lightning, flag</t>
+  </si>
+  <si>
+    <t>Command Transitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Community Sites </t>
+  </si>
+  <si>
+    <t>Traffic Impacts</t>
+  </si>
+  <si>
+    <t>Hazardous Terrain</t>
+  </si>
+  <si>
+    <t>Livestock Impacts</t>
+  </si>
+  <si>
+    <t>Law Violations</t>
+  </si>
+  <si>
+    <t>Injuries</t>
+  </si>
+  <si>
+    <t>Evacuations</t>
+  </si>
+  <si>
+    <t>Military Base Impacts</t>
+  </si>
+  <si>
+    <t>Extreme Weather</t>
+  </si>
+  <si>
+    <t>Ecological Impacts</t>
+  </si>
+  <si>
+    <t>Infrastructure Impacts</t>
+  </si>
+  <si>
+    <t>Resource Issues</t>
+  </si>
+  <si>
+    <t>Floods</t>
+  </si>
+  <si>
+    <t>Inaccurate Mapping</t>
+  </si>
+  <si>
+    <t>humidity, moisture, hot, drought</t>
+  </si>
+  <si>
+    <t>Dry Weather</t>
+  </si>
+  <si>
+    <t>Aerial Grounding</t>
+  </si>
+  <si>
+    <t>Environmental</t>
+  </si>
+  <si>
+    <t>Mission</t>
+  </si>
+  <si>
+    <t>Human Factors?</t>
+  </si>
+  <si>
+    <t>Wildland Urban Interface</t>
+  </si>
+  <si>
+    <t>jurisdiction, team, command, organization, type</t>
+  </si>
+  <si>
+    <t>terrain, rollout, snag, steep, debris, access</t>
+  </si>
+  <si>
+    <t>involve, transition, transfer</t>
+  </si>
+  <si>
+    <t>injury, hospital, injured, accident, treatment, laceration, firefighter, treat</t>
+  </si>
+  <si>
+    <t>minor, report, transport, heat, shoulder, ankle, medical, release</t>
+  </si>
+  <si>
+    <t>evacuation, evacuate, threaten, threat</t>
+  </si>
+  <si>
+    <t>low, dry, prolong</t>
+  </si>
+  <si>
+    <t>specie, habitat, animal, plant, conservation</t>
+  </si>
+  <si>
+    <t>threaten, endanger, threat, sensitive, risk, loss, impact</t>
+  </si>
+  <si>
+    <t>ground, suspend, smoke, impact, hazard, windy</t>
+  </si>
+  <si>
+    <t>resident, residence, level, notice, community, structure, subdivision, mandatory, order, effect, remain, continue, issue</t>
+  </si>
+  <si>
+    <t>unstaffed, resource, support, crew, aircraft, helicopter, engine, staff</t>
+  </si>
+  <si>
+    <t>unpredictable, extreme, erratic, strong, red, warning, warn</t>
+  </si>
+  <si>
+    <t>political, social, adjacent, community, cultural, tribal, monument, archaeological, heritage</t>
   </si>
 </sst>
 </file>
@@ -962,19 +1025,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD202B9-4913-4B48-97F7-AC087D3F80D8}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.21875" customWidth="1"/>
     <col min="2" max="2" width="25.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="9" max="9" width="5" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -984,223 +1050,324 @@
       <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="K1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>193</v>
+      </c>
+      <c r="K2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3">
+        <v>209</v>
+      </c>
+      <c r="D3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>195</v>
+      </c>
+      <c r="K3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
         <v>83</v>
       </c>
-      <c r="E4">
+      <c r="D4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>193</v>
+      </c>
+      <c r="K4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+      <c r="D5" t="s">
+        <v>133</v>
+      </c>
+      <c r="J5" t="s">
+        <v>192</v>
+      </c>
+      <c r="K5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
       </c>
-      <c r="E6">
+      <c r="D6">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J6" t="s">
+        <v>194</v>
+      </c>
+      <c r="K6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="D7">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>195</v>
+      </c>
+      <c r="K7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="C8" t="s">
         <v>90</v>
       </c>
-      <c r="E8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>153</v>
+      </c>
+      <c r="J8" t="s">
+        <v>193</v>
+      </c>
+      <c r="K8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="B9" t="s">
-        <v>166</v>
-      </c>
-      <c r="E9">
+        <v>200</v>
+      </c>
+      <c r="D9">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>194</v>
+      </c>
+      <c r="K9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>63</v>
       </c>
       <c r="B10" t="s">
         <v>64</v>
       </c>
-      <c r="E10">
+      <c r="D10">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>195</v>
+      </c>
+      <c r="K10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>195</v>
+      </c>
+      <c r="K11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>173</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12">
+        <v>208</v>
+      </c>
+      <c r="D12">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>192</v>
+      </c>
+      <c r="K12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
       <c r="B13" t="s">
-        <v>181</v>
-      </c>
-      <c r="E13">
+        <v>204</v>
+      </c>
+      <c r="D13">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>192</v>
+      </c>
+      <c r="K13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="B14" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+      <c r="D14" t="s">
+        <v>159</v>
+      </c>
+      <c r="J14" t="s">
+        <v>193</v>
+      </c>
+      <c r="K14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15">
+        <v>128</v>
+      </c>
+      <c r="J15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>146</v>
       </c>
-      <c r="B15" t="s">
-        <v>147</v>
-      </c>
-      <c r="E15">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>152</v>
-      </c>
       <c r="B16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E16">
+        <v>145</v>
+      </c>
+      <c r="D16">
         <v>135</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>193</v>
+      </c>
+      <c r="K16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" t="s">
+        <v>205</v>
+      </c>
+      <c r="C17" t="s">
         <v>172</v>
       </c>
-      <c r="B17" t="s">
-        <v>158</v>
-      </c>
-      <c r="E17">
+      <c r="J17" t="s">
+        <v>193</v>
+      </c>
+      <c r="K17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18">
         <v>144</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>186</v>
-      </c>
-      <c r="B18" t="s">
-        <v>187</v>
-      </c>
-      <c r="C18" t="s">
-        <v>188</v>
+      <c r="J18" t="s">
+        <v>192</v>
+      </c>
+      <c r="K18" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -1972,7 +2139,7 @@
         <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -1980,10 +2147,10 @@
         <v>76</v>
       </c>
       <c r="C78" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E78" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -1999,7 +2166,7 @@
         <v>78</v>
       </c>
       <c r="C80" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -2007,10 +2174,10 @@
         <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E81" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2018,10 +2185,10 @@
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E82" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -2029,10 +2196,10 @@
         <v>81</v>
       </c>
       <c r="C83" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E83" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2048,7 +2215,7 @@
         <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -2056,7 +2223,7 @@
         <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -2096,10 +2263,10 @@
         <v>89</v>
       </c>
       <c r="C91" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E91" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -2115,10 +2282,10 @@
         <v>91</v>
       </c>
       <c r="C93" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E93" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -2126,10 +2293,10 @@
         <v>92</v>
       </c>
       <c r="C94" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E94" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -2145,7 +2312,7 @@
         <v>94</v>
       </c>
       <c r="C96" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
@@ -2153,7 +2320,7 @@
         <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -2161,10 +2328,10 @@
         <v>96</v>
       </c>
       <c r="C98" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E98" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -2172,7 +2339,7 @@
         <v>97</v>
       </c>
       <c r="C99" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -2188,10 +2355,10 @@
         <v>99</v>
       </c>
       <c r="C101" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E101" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
@@ -2215,7 +2382,7 @@
         <v>102</v>
       </c>
       <c r="C104" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -2223,7 +2390,7 @@
         <v>103</v>
       </c>
       <c r="C105" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
@@ -2239,7 +2406,7 @@
         <v>105</v>
       </c>
       <c r="C107" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2247,7 +2414,7 @@
         <v>106</v>
       </c>
       <c r="C108" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -2263,7 +2430,7 @@
         <v>108</v>
       </c>
       <c r="C110" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -2279,7 +2446,7 @@
         <v>110</v>
       </c>
       <c r="C112" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -2303,7 +2470,7 @@
         <v>113</v>
       </c>
       <c r="C115" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -2311,7 +2478,7 @@
         <v>114</v>
       </c>
       <c r="C116" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -2319,7 +2486,7 @@
         <v>115</v>
       </c>
       <c r="C117" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -2343,10 +2510,10 @@
         <v>118</v>
       </c>
       <c r="C120" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E120" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2362,10 +2529,10 @@
         <v>120</v>
       </c>
       <c r="C122" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E122" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
@@ -2381,7 +2548,7 @@
         <v>122</v>
       </c>
       <c r="C124" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2389,7 +2556,7 @@
         <v>123</v>
       </c>
       <c r="C125" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -2413,7 +2580,7 @@
         <v>126</v>
       </c>
       <c r="C128" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -2421,7 +2588,7 @@
         <v>127</v>
       </c>
       <c r="C129" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -2429,10 +2596,10 @@
         <v>128</v>
       </c>
       <c r="C130" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E130" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2440,7 +2607,7 @@
         <v>129</v>
       </c>
       <c r="C131" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -2448,7 +2615,7 @@
         <v>130</v>
       </c>
       <c r="C132" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -2472,7 +2639,7 @@
         <v>133</v>
       </c>
       <c r="C135" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -2480,7 +2647,7 @@
         <v>134</v>
       </c>
       <c r="C136" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -2488,10 +2655,10 @@
         <v>135</v>
       </c>
       <c r="C137" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E137" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -2499,7 +2666,7 @@
         <v>136</v>
       </c>
       <c r="C138" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -2523,7 +2690,7 @@
         <v>139</v>
       </c>
       <c r="C141" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
@@ -2539,7 +2706,7 @@
         <v>141</v>
       </c>
       <c r="C143" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -2547,7 +2714,7 @@
         <v>142</v>
       </c>
       <c r="C144" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
@@ -2555,7 +2722,7 @@
         <v>143</v>
       </c>
       <c r="C145" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -2563,10 +2730,10 @@
         <v>144</v>
       </c>
       <c r="C146" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E146" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -2574,7 +2741,7 @@
         <v>145</v>
       </c>
       <c r="C147" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -2585,7 +2752,7 @@
         <v>40</v>
       </c>
       <c r="E148" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -2593,7 +2760,7 @@
         <v>147</v>
       </c>
       <c r="C149" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
@@ -2601,7 +2768,7 @@
         <v>148</v>
       </c>
       <c r="C150" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
@@ -2609,7 +2776,7 @@
         <v>149</v>
       </c>
       <c r="C151" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -2625,7 +2792,7 @@
         <v>151</v>
       </c>
       <c r="C153" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -2633,7 +2800,7 @@
         <v>152</v>
       </c>
       <c r="C154" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -2649,7 +2816,7 @@
         <v>154</v>
       </c>
       <c r="C156" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -2665,7 +2832,7 @@
         <v>156</v>
       </c>
       <c r="C158" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
@@ -2673,7 +2840,7 @@
         <v>157</v>
       </c>
       <c r="C159" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
@@ -2681,7 +2848,7 @@
         <v>158</v>
       </c>
       <c r="C160" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
@@ -2689,10 +2856,10 @@
         <v>159</v>
       </c>
       <c r="C161" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="E161" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated trend analysis files and results
</commit_message>
<xml_diff>
--- a/output data/hazard_interpretation_v2.xlsx
+++ b/output data/hazard_interpretation_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\output data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B452C8-9E5F-4F7F-896F-9CE7D72F2007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4E6541-5005-4CEE-AD7C-1120BD0C0F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="996" windowWidth="17280" windowHeight="10044" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hazard-focused" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="215">
   <si>
     <t>Hazard level 1 topics</t>
   </si>
@@ -262,9 +262,6 @@
     <t>evacuation/public impacts</t>
   </si>
   <si>
-    <t>difficult, erratic, problem, snag, thick timber, etc</t>
-  </si>
-  <si>
     <t>terrain/condition related; not the hazard types we want</t>
   </si>
   <si>
@@ -283,9 +280,6 @@
     <t>mixed</t>
   </si>
   <si>
-    <t>highway, road, close, traffic, closure, campground, public, visitor,  impact, access,  limited, safety, evacuate</t>
-  </si>
-  <si>
     <t>reopen, open</t>
   </si>
   <si>
@@ -460,9 +454,6 @@
     <t>flood, flashflood</t>
   </si>
   <si>
-    <t>flash, risk, potential</t>
-  </si>
-  <si>
     <t>mixed, international border</t>
   </si>
   <si>
@@ -562,18 +553,9 @@
     <t>Command Transitions</t>
   </si>
   <si>
-    <t xml:space="preserve">Community Sites </t>
-  </si>
-  <si>
-    <t>Traffic Impacts</t>
-  </si>
-  <si>
     <t>Hazardous Terrain</t>
   </si>
   <si>
-    <t>Livestock Impacts</t>
-  </si>
-  <si>
     <t>Law Violations</t>
   </si>
   <si>
@@ -583,18 +565,9 @@
     <t>Evacuations</t>
   </si>
   <si>
-    <t>Military Base Impacts</t>
-  </si>
-  <si>
     <t>Extreme Weather</t>
   </si>
   <si>
-    <t>Ecological Impacts</t>
-  </si>
-  <si>
-    <t>Infrastructure Impacts</t>
-  </si>
-  <si>
     <t>Resource Issues</t>
   </si>
   <si>
@@ -665,6 +638,48 @@
   </si>
   <si>
     <t>political, social, adjacent, community, cultural, tribal, monument, archaeological, heritage</t>
+  </si>
+  <si>
+    <t>Cultural Resources</t>
+  </si>
+  <si>
+    <t>Traffic</t>
+  </si>
+  <si>
+    <t>Livestock</t>
+  </si>
+  <si>
+    <t>Military Base</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+  </si>
+  <si>
+    <t>Ecological</t>
+  </si>
+  <si>
+    <t>flash, risk, potential, chance</t>
+  </si>
+  <si>
+    <t>difficult, erratic, problem, snag, thick, timber</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Law Violation</t>
+  </si>
+  <si>
+    <t>Evacuation</t>
+  </si>
+  <si>
+    <t>highway, road, close, traffic, closure, campground, public, visitor,  impact, access,  limited, safety</t>
+  </si>
+  <si>
+    <t>Command Transfer</t>
+  </si>
+  <si>
+    <t>Containment Difficulty</t>
   </si>
 </sst>
 </file>
@@ -1027,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD202B9-4913-4B48-97F7-AC087D3F80D8}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1071,73 +1086,73 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="K2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="K3" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" t="s">
         <v>166</v>
       </c>
-      <c r="B4" t="s">
-        <v>169</v>
-      </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D4">
         <v>6</v>
       </c>
       <c r="J4" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="K4" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J5" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="K5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1151,64 +1166,64 @@
         <v>21</v>
       </c>
       <c r="J6" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="K6" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D7">
         <v>23</v>
       </c>
       <c r="J7" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="K7" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B8" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J8" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="K8" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D9">
         <v>34</v>
       </c>
       <c r="J9" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="K9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1222,152 +1237,152 @@
         <v>52</v>
       </c>
       <c r="J10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="K10" t="s">
-        <v>182</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J11" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="K11" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D12">
         <v>76</v>
       </c>
       <c r="J12" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="K12" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B13" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D13">
         <v>80</v>
       </c>
       <c r="J13" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="K13" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D14" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J14" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="K14" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>207</v>
       </c>
       <c r="D15">
         <v>128</v>
       </c>
       <c r="J15" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="K15" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D16">
         <v>135</v>
       </c>
       <c r="J16" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="K16" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B17" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C17" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J17" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="K17" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B18" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D18">
         <v>144</v>
       </c>
       <c r="J18" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="K18" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1380,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E799D7D2-7755-4A40-8FAC-FBB6E32500C5}">
   <dimension ref="A1:R161"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A162" sqref="A162"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="R161" sqref="R161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1515,6 +1530,12 @@
       <c r="M7" t="s">
         <v>17</v>
       </c>
+      <c r="P7" t="s">
+        <v>186</v>
+      </c>
+      <c r="R7" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -1529,19 +1550,31 @@
       <c r="M8" t="s">
         <v>20</v>
       </c>
+      <c r="P8" t="s">
+        <v>184</v>
+      </c>
+      <c r="R8" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>208</v>
       </c>
       <c r="M9" t="s">
         <v>20</v>
+      </c>
+      <c r="P9" t="s">
+        <v>209</v>
+      </c>
+      <c r="R9" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -1549,7 +1582,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -1571,7 +1604,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -1609,7 +1642,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1620,7 +1653,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1628,7 +1661,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1636,7 +1669,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1644,7 +1677,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1652,7 +1685,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1662,8 +1695,14 @@
       <c r="E22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P22" t="s">
+        <v>209</v>
+      </c>
+      <c r="R22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1673,8 +1712,14 @@
       <c r="E23" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P23" t="s">
+        <v>186</v>
+      </c>
+      <c r="R23" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1682,7 +1727,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1692,8 +1737,14 @@
       <c r="E25" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P25" t="s">
+        <v>186</v>
+      </c>
+      <c r="R25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1701,7 +1752,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1714,8 +1765,14 @@
       <c r="N27" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P27" t="s">
+        <v>184</v>
+      </c>
+      <c r="R27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1723,7 +1780,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1731,7 +1788,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1739,7 +1796,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1747,7 +1804,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1755,7 +1812,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1763,7 +1820,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1771,7 +1828,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1781,8 +1838,14 @@
       <c r="E35" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P35" t="s">
+        <v>209</v>
+      </c>
+      <c r="R35" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1792,8 +1855,14 @@
       <c r="E36" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P36" t="s">
+        <v>184</v>
+      </c>
+      <c r="R36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1801,7 +1870,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1809,7 +1878,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1817,7 +1886,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1825,7 +1894,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1833,7 +1902,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1841,7 +1910,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1849,7 +1918,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1857,7 +1926,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1865,7 +1934,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1873,7 +1942,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1883,8 +1952,14 @@
       <c r="E47" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P47" t="s">
+        <v>184</v>
+      </c>
+      <c r="R47" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1892,7 +1967,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1900,7 +1975,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1908,7 +1983,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1916,7 +1991,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1924,7 +1999,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1932,7 +2007,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1942,8 +2017,14 @@
       <c r="E54" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="P54" t="s">
+        <v>186</v>
+      </c>
+      <c r="R54" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1951,7 +2032,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1959,7 +2040,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1967,7 +2048,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1975,7 +2056,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1983,7 +2064,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1991,7 +2072,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2002,7 +2083,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -2010,39 +2091,39 @@
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="C66" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -2050,7 +2131,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -2058,7 +2139,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -2066,7 +2147,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -2074,59 +2155,83 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E71" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="P71" t="s">
+        <v>184</v>
+      </c>
+      <c r="R71" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E72" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="P72" t="s">
+        <v>186</v>
+      </c>
+      <c r="R72" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E73" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="P73" t="s">
+        <v>186</v>
+      </c>
+      <c r="R73" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
       <c r="C74" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E74" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="P74" t="s">
+        <v>184</v>
+      </c>
+      <c r="R74" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -2134,115 +2239,139 @@
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
       <c r="C78" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E78" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="P78" t="s">
+        <v>209</v>
+      </c>
+      <c r="R78" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
       <c r="C79" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
       <c r="C80" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E81" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="P81" t="s">
+        <v>184</v>
+      </c>
+      <c r="R81" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E82" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="P82" t="s">
+        <v>209</v>
+      </c>
+      <c r="R82" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
       <c r="C83" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E83" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="P83" t="s">
+        <v>209</v>
+      </c>
+      <c r="R83" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
       <c r="C84" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
       <c r="C87" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
       <c r="C88" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -2250,26 +2379,32 @@
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
       <c r="C90" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
       <c r="C91" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E91" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="P91" t="s">
+        <v>209</v>
+      </c>
+      <c r="R91" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -2277,72 +2412,84 @@
         <v>72</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
       <c r="C93" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E93" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
       <c r="C94" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E94" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="P94" t="s">
+        <v>209</v>
+      </c>
+      <c r="R94" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
       <c r="C95" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
       <c r="C96" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>96</v>
       </c>
       <c r="C98" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E98" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="P98" t="s">
+        <v>186</v>
+      </c>
+      <c r="R98" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>97</v>
       </c>
       <c r="C99" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>98</v>
       </c>
@@ -2350,18 +2497,24 @@
         <v>72</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>99</v>
       </c>
       <c r="C101" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E101" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="P101" t="s">
+        <v>184</v>
+      </c>
+      <c r="R101" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>100</v>
       </c>
@@ -2369,31 +2522,31 @@
         <v>72</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>101</v>
       </c>
       <c r="C103" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>102</v>
       </c>
       <c r="C104" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>103</v>
       </c>
       <c r="C105" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>104</v>
       </c>
@@ -2401,23 +2554,23 @@
         <v>72</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>105</v>
       </c>
       <c r="C107" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>106</v>
       </c>
       <c r="C108" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>107</v>
       </c>
@@ -2425,15 +2578,15 @@
         <v>72</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>108</v>
       </c>
       <c r="C110" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>109</v>
       </c>
@@ -2441,15 +2594,15 @@
         <v>72</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>110</v>
       </c>
       <c r="C112" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>111</v>
       </c>
@@ -2457,7 +2610,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>112</v>
       </c>
@@ -2465,31 +2618,31 @@
         <v>72</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>113</v>
       </c>
       <c r="C115" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>114</v>
       </c>
       <c r="C116" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>115</v>
       </c>
       <c r="C117" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>116</v>
       </c>
@@ -2497,7 +2650,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>117</v>
       </c>
@@ -2505,18 +2658,18 @@
         <v>72</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>118</v>
       </c>
       <c r="C120" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E120" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>119</v>
       </c>
@@ -2524,18 +2677,24 @@
         <v>72</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>120</v>
       </c>
       <c r="C122" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E122" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+      <c r="P122" t="s">
+        <v>209</v>
+      </c>
+      <c r="R122" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>121</v>
       </c>
@@ -2543,23 +2702,23 @@
         <v>72</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>122</v>
       </c>
       <c r="C124" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>123</v>
       </c>
       <c r="C125" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>124</v>
       </c>
@@ -2567,7 +2726,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>125</v>
       </c>
@@ -2575,58 +2734,64 @@
         <v>72</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>126</v>
       </c>
       <c r="C128" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>127</v>
       </c>
       <c r="C129" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>128</v>
       </c>
       <c r="C130" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E130" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+      <c r="P130" t="s">
+        <v>209</v>
+      </c>
+      <c r="R130" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>129</v>
       </c>
       <c r="C131" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>130</v>
       </c>
       <c r="C132" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>131</v>
       </c>
       <c r="C133" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>132</v>
       </c>
@@ -2634,42 +2799,48 @@
         <v>43</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>133</v>
       </c>
       <c r="C135" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>134</v>
       </c>
       <c r="C136" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>135</v>
       </c>
       <c r="C137" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E137" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="P137" t="s">
+        <v>184</v>
+      </c>
+      <c r="R137" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>136</v>
       </c>
       <c r="C138" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>137</v>
       </c>
@@ -2677,7 +2848,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>138</v>
       </c>
@@ -2685,66 +2856,66 @@
         <v>52</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>139</v>
       </c>
       <c r="C141" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>140</v>
       </c>
       <c r="C142" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>141</v>
       </c>
       <c r="C143" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>142</v>
       </c>
       <c r="C144" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>143</v>
       </c>
       <c r="C145" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>144</v>
       </c>
       <c r="C146" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E146" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>145</v>
       </c>
       <c r="C147" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>146</v>
       </c>
@@ -2752,34 +2923,40 @@
         <v>40</v>
       </c>
       <c r="E148" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="P148" t="s">
+        <v>184</v>
+      </c>
+      <c r="R148" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>147</v>
       </c>
       <c r="C149" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>148</v>
       </c>
       <c r="C150" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>149</v>
       </c>
       <c r="C151" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>150</v>
       </c>
@@ -2787,23 +2964,23 @@
         <v>72</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>151</v>
       </c>
       <c r="C153" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>152</v>
       </c>
       <c r="C154" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>153</v>
       </c>
@@ -2811,15 +2988,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>154</v>
       </c>
       <c r="C156" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>155</v>
       </c>
@@ -2827,39 +3004,45 @@
         <v>72</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>156</v>
       </c>
       <c r="C158" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>157</v>
       </c>
       <c r="C159" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>158</v>
       </c>
       <c r="C160" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>159</v>
       </c>
       <c r="C161" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E161" t="s">
-        <v>165</v>
+        <v>162</v>
+      </c>
+      <c r="P161" t="s">
+        <v>184</v>
+      </c>
+      <c r="R161" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added hazard extraction accuracy results, edited hazard extraction to improve accuracy, adjusted test file accordingly
</commit_message>
<xml_diff>
--- a/output data/hazard_interpretation_v2.xlsx
+++ b/output data/hazard_interpretation_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\output data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4E6541-5005-4CEE-AD7C-1120BD0C0F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52C40D3-1981-4393-A147-1828DA2FF09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
+    <workbookView xWindow="14688" yWindow="1164" windowWidth="17280" windowHeight="10044" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hazard-focused" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="216">
   <si>
     <t>Hazard level 1 topics</t>
   </si>
@@ -226,12 +226,6 @@
     <t>military, training, impact, unexploded,, proximity, notice</t>
   </si>
   <si>
-    <t>military, unexploded, national</t>
-  </si>
-  <si>
-    <t>training, present, ordinance, guard</t>
-  </si>
-  <si>
     <t>command description</t>
   </si>
   <si>
@@ -280,9 +274,6 @@
     <t>mixed</t>
   </si>
   <si>
-    <t>reopen, open</t>
-  </si>
-  <si>
     <t>redundant, traffic</t>
   </si>
   <si>
@@ -301,9 +292,6 @@
     <t>70, 71</t>
   </si>
   <si>
-    <t>lift, return, reopen, open</t>
-  </si>
-  <si>
     <t>mixed, team transition</t>
   </si>
   <si>
@@ -331,9 +319,6 @@
     <t xml:space="preserve"> limited, suppression, limit, difficulty, minimal, mist, action, staff, access, country, difficult, steep, fuel, full, infrastucture, pose, milne, terrain, concern, spread</t>
   </si>
   <si>
-    <t>grazing, pasture, threaten, concern, risk, threat</t>
-  </si>
-  <si>
     <t>mixed, some endangered species</t>
   </si>
   <si>
@@ -379,9 +364,6 @@
     <t>utility, company, residential, tower, transmission, inspection, powerlines, hazard, resident, local, public, pole, operational</t>
   </si>
   <si>
-    <t>restore</t>
-  </si>
-  <si>
     <t>rain, not a hazard</t>
   </si>
   <si>
@@ -391,9 +373,6 @@
     <t>unstaffed, lack, allotment, engage, unable</t>
   </si>
   <si>
-    <t>release, demob, demobilization</t>
-  </si>
-  <si>
     <t>reports about findings from infrared flight, not hazard</t>
   </si>
   <si>
@@ -448,9 +427,6 @@
     <t>flood, heavy, storm, water, potential, damage</t>
   </si>
   <si>
-    <t>cattle, buffalo, grow, allotment, ranch, sheep, livestock</t>
-  </si>
-  <si>
     <t>flood, flashflood</t>
   </si>
   <si>
@@ -463,9 +439,6 @@
     <t>mapping, accurate, acreage, reduction, change, decrease, acre, reduce, size, database, reflect, adjustment, suite</t>
   </si>
   <si>
-    <t>reflect, accurate, adjustment, change, reflect</t>
-  </si>
-  <si>
     <t>mapping, map</t>
   </si>
   <si>
@@ -535,18 +508,9 @@
     <t>infrastructure, utility, powerline, water, electric, pipeline, powerlines, watershed, pole, power, gas</t>
   </si>
   <si>
-    <t>closure, remain, remains, close, block, continue, impact, access, limit, limited</t>
-  </si>
-  <si>
     <t>lack, need, shortage, minimal, share, necessary, limited, limit, fatigue</t>
   </si>
   <si>
-    <t>aircraft, heli, helicopter, aerial, tanker, copter</t>
-  </si>
-  <si>
-    <t>resume</t>
-  </si>
-  <si>
     <t>weather, behavior, wind, thunderstorm, storm, gusty, lightning, flag</t>
   </si>
   <si>
@@ -592,9 +556,6 @@
     <t>Mission</t>
   </si>
   <si>
-    <t>Human Factors?</t>
-  </si>
-  <si>
     <t>Wildland Urban Interface</t>
   </si>
   <si>
@@ -625,9 +586,6 @@
     <t>threaten, endanger, threat, sensitive, risk, loss, impact</t>
   </si>
   <si>
-    <t>ground, suspend, smoke, impact, hazard, windy</t>
-  </si>
-  <si>
     <t>resident, residence, level, notice, community, structure, subdivision, mandatory, order, effect, remain, continue, issue</t>
   </si>
   <si>
@@ -680,6 +638,51 @@
   </si>
   <si>
     <t>Containment Difficulty</t>
+  </si>
+  <si>
+    <t>smoke</t>
+  </si>
+  <si>
+    <t>reopen, open, lift</t>
+  </si>
+  <si>
+    <t>closure, remain, remains, close, block, impact, access, limit, limited</t>
+  </si>
+  <si>
+    <t>reverse</t>
+  </si>
+  <si>
+    <t>cattle, buffalo, allotment, ranch, sheep, livestock</t>
+  </si>
+  <si>
+    <t>lift, return, reopen, open, reduce</t>
+  </si>
+  <si>
+    <t>military, unexploded</t>
+  </si>
+  <si>
+    <t>restore, tender, diminished</t>
+  </si>
+  <si>
+    <t>resume, drop, lack, lift</t>
+  </si>
+  <si>
+    <t>training, present, ordinance, proximity, activity, active, base, area</t>
+  </si>
+  <si>
+    <t>grazing, pasture, threaten, concern, risk, threat, private, area, evacuate, evacuation, order</t>
+  </si>
+  <si>
+    <t>release, demob, demobilization, demobilize, progress</t>
+  </si>
+  <si>
+    <t>aircraft, heli, helicopter, aerial, tanker, copter, ground</t>
+  </si>
+  <si>
+    <t>suspend, smoke, hazard, windy, wind, suspendsion, mechanical, problem, due</t>
+  </si>
+  <si>
+    <t>reflect, accurate, adjustment, change, reflect, inaccurate</t>
   </si>
 </sst>
 </file>
@@ -1042,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD202B9-4913-4B48-97F7-AC087D3F80D8}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1086,303 +1089,309 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D2" t="s">
-        <v>91</v>
+        <v>203</v>
+      </c>
+      <c r="C2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
       </c>
       <c r="J2" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="K2" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
+        <v>176</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
       </c>
       <c r="J3" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="K3" t="s">
-        <v>201</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" t="s">
+        <v>172</v>
+      </c>
+      <c r="K4" t="s">
         <v>163</v>
-      </c>
-      <c r="B4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="J4" t="s">
-        <v>184</v>
-      </c>
-      <c r="K4" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" t="s">
-        <v>131</v>
+        <v>215</v>
+      </c>
+      <c r="D5">
+        <v>135</v>
       </c>
       <c r="J5" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="K5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6">
-        <v>21</v>
+        <v>214</v>
+      </c>
+      <c r="C6" t="s">
+        <v>209</v>
       </c>
       <c r="J6" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="K6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>184</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7">
-        <v>23</v>
+        <v>157</v>
+      </c>
+      <c r="C7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" t="s">
+        <v>147</v>
       </c>
       <c r="J7" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="K7" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" t="s">
-        <v>150</v>
+        <v>178</v>
+      </c>
+      <c r="D8">
+        <v>34</v>
       </c>
       <c r="J8" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="K8" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>191</v>
+        <v>186</v>
+      </c>
+      <c r="C9" t="s">
+        <v>201</v>
       </c>
       <c r="D9">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="J9" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="K9" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>205</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>211</v>
       </c>
       <c r="D10">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="K10" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" t="s">
-        <v>87</v>
+        <v>204</v>
+      </c>
+      <c r="D11">
+        <v>21</v>
       </c>
       <c r="J11" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="K11" t="s">
-        <v>205</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="B12" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="D12">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="J12" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="K12" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s">
-        <v>195</v>
-      </c>
-      <c r="D13">
-        <v>80</v>
+        <v>155</v>
+      </c>
+      <c r="C13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
       </c>
       <c r="J13" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="K13" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>198</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
-        <v>167</v>
-      </c>
-      <c r="C14" t="s">
-        <v>118</v>
-      </c>
-      <c r="D14" t="s">
-        <v>156</v>
+        <v>185</v>
+      </c>
+      <c r="D14">
+        <v>76</v>
       </c>
       <c r="J14" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="K14" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="D15">
-        <v>128</v>
+        <v>80</v>
       </c>
       <c r="J15" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="K15" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
-      </c>
-      <c r="D16">
-        <v>135</v>
+        <v>123</v>
+      </c>
+      <c r="D16" t="s">
+        <v>124</v>
       </c>
       <c r="J16" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="K16" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>196</v>
-      </c>
-      <c r="C17" t="s">
-        <v>169</v>
+        <v>193</v>
+      </c>
+      <c r="D17">
+        <v>128</v>
       </c>
       <c r="J17" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="K17" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" t="s">
         <v>180</v>
-      </c>
-      <c r="B18" t="s">
-        <v>193</v>
       </c>
       <c r="D18">
         <v>144</v>
       </c>
       <c r="J18" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="K18" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1395,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E799D7D2-7755-4A40-8FAC-FBB6E32500C5}">
   <dimension ref="A1:R161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="R161" sqref="R161"/>
+    <sheetView topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="I141" sqref="I141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1411,7 +1420,7 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -1449,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -1466,7 +1475,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -1483,7 +1492,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -1497,7 +1506,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -1511,7 +1520,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
@@ -1531,10 +1540,10 @@
         <v>17</v>
       </c>
       <c r="P7" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="R7" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -1542,7 +1551,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
@@ -1551,10 +1560,10 @@
         <v>20</v>
       </c>
       <c r="P8" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="R8" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -1562,19 +1571,19 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="M9" t="s">
         <v>20</v>
       </c>
       <c r="P9" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="R9" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -1582,7 +1591,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -1593,7 +1602,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -1604,7 +1613,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -1615,7 +1624,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -1696,10 +1705,10 @@
         <v>31</v>
       </c>
       <c r="P22" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="R22" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
@@ -1713,10 +1722,10 @@
         <v>32</v>
       </c>
       <c r="P23" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="R23" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
@@ -1738,10 +1747,10 @@
         <v>38</v>
       </c>
       <c r="P25" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="R25" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
@@ -1766,10 +1775,10 @@
         <v>42</v>
       </c>
       <c r="P27" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="R27" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
@@ -1839,10 +1848,10 @@
         <v>48</v>
       </c>
       <c r="P35" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="R35" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
@@ -1856,10 +1865,10 @@
         <v>50</v>
       </c>
       <c r="P36" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="R36" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
@@ -1953,10 +1962,10 @@
         <v>56</v>
       </c>
       <c r="P47" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="R47" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
@@ -2018,10 +2027,10 @@
         <v>62</v>
       </c>
       <c r="P54" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="R54" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
@@ -2029,7 +2038,7 @@
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.3">
@@ -2045,7 +2054,7 @@
         <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
@@ -2061,7 +2070,7 @@
         <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
@@ -2069,7 +2078,7 @@
         <v>58</v>
       </c>
       <c r="C60" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">
@@ -2077,10 +2086,10 @@
         <v>59</v>
       </c>
       <c r="C61" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E61" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.3">
@@ -2096,7 +2105,7 @@
         <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.3">
@@ -2104,7 +2113,7 @@
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.3">
@@ -2112,7 +2121,7 @@
         <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.3">
@@ -2120,7 +2129,7 @@
         <v>64</v>
       </c>
       <c r="C66" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.3">
@@ -2128,7 +2137,7 @@
         <v>65</v>
       </c>
       <c r="C67" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.3">
@@ -2144,7 +2153,7 @@
         <v>67</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.3">
@@ -2152,7 +2161,7 @@
         <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.3">
@@ -2160,16 +2169,16 @@
         <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E71" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="P71" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="R71" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.3">
@@ -2177,16 +2186,16 @@
         <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E72" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="P72" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="R72" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.3">
@@ -2194,16 +2203,16 @@
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E73" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="P73" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="R73" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.3">
@@ -2211,16 +2220,16 @@
         <v>72</v>
       </c>
       <c r="C74" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E74" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="P74" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="R74" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.3">
@@ -2228,7 +2237,7 @@
         <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.3">
@@ -2236,7 +2245,7 @@
         <v>74</v>
       </c>
       <c r="C76" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.3">
@@ -2244,7 +2253,7 @@
         <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.3">
@@ -2252,16 +2261,16 @@
         <v>76</v>
       </c>
       <c r="C78" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E78" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="P78" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="R78" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.3">
@@ -2269,7 +2278,7 @@
         <v>77</v>
       </c>
       <c r="C79" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.3">
@@ -2277,7 +2286,7 @@
         <v>78</v>
       </c>
       <c r="C80" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.3">
@@ -2285,16 +2294,16 @@
         <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E81" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="P81" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="R81" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.3">
@@ -2302,16 +2311,16 @@
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E82" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P82" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="R82" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.3">
@@ -2319,16 +2328,16 @@
         <v>81</v>
       </c>
       <c r="C83" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E83" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="P83" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="R83" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.3">
@@ -2336,7 +2345,7 @@
         <v>82</v>
       </c>
       <c r="C84" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.3">
@@ -2344,7 +2353,7 @@
         <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.3">
@@ -2352,7 +2361,7 @@
         <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.3">
@@ -2360,7 +2369,7 @@
         <v>85</v>
       </c>
       <c r="C87" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.3">
@@ -2368,7 +2377,7 @@
         <v>86</v>
       </c>
       <c r="C88" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.3">
@@ -2384,7 +2393,7 @@
         <v>88</v>
       </c>
       <c r="C90" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.3">
@@ -2392,16 +2401,16 @@
         <v>89</v>
       </c>
       <c r="C91" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E91" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="P91" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="R91" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.3">
@@ -2409,7 +2418,7 @@
         <v>90</v>
       </c>
       <c r="C92" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.3">
@@ -2417,10 +2426,10 @@
         <v>91</v>
       </c>
       <c r="C93" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E93" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.3">
@@ -2428,16 +2437,16 @@
         <v>92</v>
       </c>
       <c r="C94" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E94" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="P94" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="R94" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.3">
@@ -2445,7 +2454,7 @@
         <v>93</v>
       </c>
       <c r="C95" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.3">
@@ -2453,7 +2462,7 @@
         <v>94</v>
       </c>
       <c r="C96" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.3">
@@ -2461,7 +2470,7 @@
         <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.3">
@@ -2469,16 +2478,16 @@
         <v>96</v>
       </c>
       <c r="C98" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E98" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="P98" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="R98" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.3">
@@ -2486,7 +2495,7 @@
         <v>97</v>
       </c>
       <c r="C99" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.3">
@@ -2494,7 +2503,7 @@
         <v>98</v>
       </c>
       <c r="C100" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.3">
@@ -2502,16 +2511,16 @@
         <v>99</v>
       </c>
       <c r="C101" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E101" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="P101" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="R101" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.3">
@@ -2519,7 +2528,7 @@
         <v>100</v>
       </c>
       <c r="C102" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.3">
@@ -2527,7 +2536,7 @@
         <v>101</v>
       </c>
       <c r="C103" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.3">
@@ -2535,7 +2544,7 @@
         <v>102</v>
       </c>
       <c r="C104" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.3">
@@ -2543,7 +2552,7 @@
         <v>103</v>
       </c>
       <c r="C105" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.3">
@@ -2551,7 +2560,7 @@
         <v>104</v>
       </c>
       <c r="C106" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.3">
@@ -2559,7 +2568,7 @@
         <v>105</v>
       </c>
       <c r="C107" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.3">
@@ -2567,7 +2576,7 @@
         <v>106</v>
       </c>
       <c r="C108" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.3">
@@ -2575,7 +2584,7 @@
         <v>107</v>
       </c>
       <c r="C109" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.3">
@@ -2583,7 +2592,7 @@
         <v>108</v>
       </c>
       <c r="C110" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.3">
@@ -2591,7 +2600,7 @@
         <v>109</v>
       </c>
       <c r="C111" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.3">
@@ -2599,7 +2608,7 @@
         <v>110</v>
       </c>
       <c r="C112" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.3">
@@ -2615,7 +2624,7 @@
         <v>112</v>
       </c>
       <c r="C114" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.3">
@@ -2623,7 +2632,7 @@
         <v>113</v>
       </c>
       <c r="C115" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.3">
@@ -2631,7 +2640,7 @@
         <v>114</v>
       </c>
       <c r="C116" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.3">
@@ -2639,7 +2648,7 @@
         <v>115</v>
       </c>
       <c r="C117" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.3">
@@ -2647,7 +2656,7 @@
         <v>116</v>
       </c>
       <c r="C118" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.3">
@@ -2655,7 +2664,7 @@
         <v>117</v>
       </c>
       <c r="C119" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.3">
@@ -2663,10 +2672,10 @@
         <v>118</v>
       </c>
       <c r="C120" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E120" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.3">
@@ -2674,7 +2683,7 @@
         <v>119</v>
       </c>
       <c r="C121" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.3">
@@ -2682,16 +2691,16 @@
         <v>120</v>
       </c>
       <c r="C122" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E122" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="P122" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="R122" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.3">
@@ -2699,7 +2708,7 @@
         <v>121</v>
       </c>
       <c r="C123" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.3">
@@ -2707,7 +2716,7 @@
         <v>122</v>
       </c>
       <c r="C124" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.3">
@@ -2715,7 +2724,7 @@
         <v>123</v>
       </c>
       <c r="C125" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.3">
@@ -2723,7 +2732,7 @@
         <v>124</v>
       </c>
       <c r="C126" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.3">
@@ -2731,7 +2740,7 @@
         <v>125</v>
       </c>
       <c r="C127" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.3">
@@ -2739,7 +2748,7 @@
         <v>126</v>
       </c>
       <c r="C128" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.3">
@@ -2747,7 +2756,7 @@
         <v>127</v>
       </c>
       <c r="C129" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.3">
@@ -2755,16 +2764,16 @@
         <v>128</v>
       </c>
       <c r="C130" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E130" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="P130" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="R130" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.3">
@@ -2772,7 +2781,7 @@
         <v>129</v>
       </c>
       <c r="C131" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.3">
@@ -2780,7 +2789,7 @@
         <v>130</v>
       </c>
       <c r="C132" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.3">
@@ -2788,7 +2797,7 @@
         <v>131</v>
       </c>
       <c r="C133" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.3">
@@ -2804,7 +2813,7 @@
         <v>133</v>
       </c>
       <c r="C135" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.3">
@@ -2812,7 +2821,7 @@
         <v>134</v>
       </c>
       <c r="C136" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.3">
@@ -2820,16 +2829,16 @@
         <v>135</v>
       </c>
       <c r="C137" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E137" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="P137" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="R137" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.3">
@@ -2837,7 +2846,7 @@
         <v>136</v>
       </c>
       <c r="C138" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.3">
@@ -2861,7 +2870,7 @@
         <v>139</v>
       </c>
       <c r="C141" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.3">
@@ -2869,7 +2878,7 @@
         <v>140</v>
       </c>
       <c r="C142" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.3">
@@ -2877,7 +2886,7 @@
         <v>141</v>
       </c>
       <c r="C143" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.3">
@@ -2885,7 +2894,7 @@
         <v>142</v>
       </c>
       <c r="C144" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.3">
@@ -2893,7 +2902,7 @@
         <v>143</v>
       </c>
       <c r="C145" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.3">
@@ -2901,10 +2910,10 @@
         <v>144</v>
       </c>
       <c r="C146" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E146" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.3">
@@ -2912,7 +2921,7 @@
         <v>145</v>
       </c>
       <c r="C147" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.3">
@@ -2923,13 +2932,13 @@
         <v>40</v>
       </c>
       <c r="E148" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="P148" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="R148" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.3">
@@ -2937,7 +2946,7 @@
         <v>147</v>
       </c>
       <c r="C149" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.3">
@@ -2945,7 +2954,7 @@
         <v>148</v>
       </c>
       <c r="C150" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.3">
@@ -2953,7 +2962,7 @@
         <v>149</v>
       </c>
       <c r="C151" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.3">
@@ -2961,7 +2970,7 @@
         <v>150</v>
       </c>
       <c r="C152" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.3">
@@ -2969,7 +2978,7 @@
         <v>151</v>
       </c>
       <c r="C153" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.3">
@@ -2977,7 +2986,7 @@
         <v>152</v>
       </c>
       <c r="C154" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.3">
@@ -2993,7 +3002,7 @@
         <v>154</v>
       </c>
       <c r="C156" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.3">
@@ -3001,7 +3010,7 @@
         <v>155</v>
       </c>
       <c r="C157" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.3">
@@ -3009,7 +3018,7 @@
         <v>156</v>
       </c>
       <c r="C158" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.3">
@@ -3017,7 +3026,7 @@
         <v>157</v>
       </c>
       <c r="C159" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.3">
@@ -3025,7 +3034,7 @@
         <v>158</v>
       </c>
       <c r="C160" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.3">
@@ -3033,16 +3042,16 @@
         <v>159</v>
       </c>
       <c r="C161" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E161" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="P161" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="R161" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>